<commit_message>
update NIST AI RMF
add description of functions
</commit_message>
<xml_diff>
--- a/tools/nist/ai-rmf/nist-ai-rmf-1.0.xlsx
+++ b/tools/nist/ai-rmf/nist-ai-rmf-1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/ai-rmf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592F8779-A243-A644-9E06-2811505DADF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1638E3D2-9BC1-1A41-BA88-7AE9DDC06733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{3035E98F-1604-1D41-B00F-0B1EACA0BE02}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="236">
   <si>
     <t>Policies, processes, procedures, and practices across the organization related to the mapping, measuring, and managing of AI risks are in place, transparent, and implemented effectively.</t>
   </si>
@@ -752,6 +752,18 @@
   </si>
   <si>
     <t>Preamble</t>
+  </si>
+  <si>
+    <t>A culture of risk management is cultivated and present.</t>
+  </si>
+  <si>
+    <t>Context is recognized and risks related to context are identified.</t>
+  </si>
+  <si>
+    <t>Identified risks are assessed, analyzed, or tracked.</t>
+  </si>
+  <si>
+    <t>Risks are prioritized and acted upon based on a projected impact.</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B503A46-E291-FE4B-9A82-51E0E3787366}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B92" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>1</v>
@@ -1349,7 +1361,9 @@
         <v>20</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -1778,7 +1792,9 @@
         <v>51</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
@@ -2179,7 +2195,9 @@
         <v>92</v>
       </c>
       <c r="D62" s="2"/>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
@@ -2627,7 +2645,9 @@
         <v>129</v>
       </c>
       <c r="D94" s="2"/>
-      <c r="E94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>

</xml_diff>